<commit_message>
added tabview for search results, todo: fix recursion error
</commit_message>
<xml_diff>
--- a/app/assets/conjugation_data.xlsx
+++ b/app/assets/conjugation_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5107a456074413f0/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5107a456074413f0/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{D3FC7C82-F881-4D8C-B0D0-4E39874438CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06781051-95D0-4210-B821-33644FE15821}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{D3FC7C82-F881-4D8C-B0D0-4E39874438CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7925971-AD20-4D6E-8292-F9AB1F14767D}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{7AE52FB5-DE8E-4E3C-A727-8474DACC6D33}"/>
+    <workbookView xWindow="1750" yWindow="1750" windowWidth="14400" windowHeight="7290" xr2:uid="{7AE52FB5-DE8E-4E3C-A727-8474DACC6D33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
   <si>
     <t>EnglishInfinitive</t>
   </si>
@@ -301,6 +301,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -620,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3FBA9C8-FE08-41FF-B674-AEE124320630}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -856,6 +860,11 @@
         <v>70</v>
       </c>
     </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.75">
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>